<commit_message>
still working on combat
</commit_message>
<xml_diff>
--- a/Resources/Game_Data.xlsx
+++ b/Resources/Game_Data.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Skills_Bonus" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621" calcMode="manual" iterate="1"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -2436,11 +2435,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="266762880"/>
-        <c:axId val="266772864"/>
+        <c:axId val="139123328"/>
+        <c:axId val="139202944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="266762880"/>
+        <c:axId val="139123328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2449,7 +2448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="266772864"/>
+        <c:crossAx val="139202944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2457,7 +2456,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="266772864"/>
+        <c:axId val="139202944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2468,7 +2467,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="266762880"/>
+        <c:crossAx val="139123328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3805,11 +3804,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="270562432"/>
-        <c:axId val="270563968"/>
+        <c:axId val="139588736"/>
+        <c:axId val="139590272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="270562432"/>
+        <c:axId val="139588736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3819,7 +3818,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="270563968"/>
+        <c:crossAx val="139590272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3827,7 +3826,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="270563968"/>
+        <c:axId val="139590272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3838,14 +3837,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="270562432"/>
+        <c:crossAx val="139588736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6330,11 +6328,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="294464896"/>
-        <c:axId val="294466688"/>
+        <c:axId val="139627904"/>
+        <c:axId val="139633792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="294464896"/>
+        <c:axId val="139627904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6343,7 +6341,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="294466688"/>
+        <c:crossAx val="139633792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6351,7 +6349,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="294466688"/>
+        <c:axId val="139633792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6362,13 +6360,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="294464896"/>
+        <c:crossAx val="139627904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -26386,8 +26385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29974,7 +29973,7 @@
   <dimension ref="A1:O403"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30101,11 +30100,11 @@
         <v>5</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:O4" si="1">E3+5</f>
+        <f>E3+5</f>
         <v>5</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="E4:O4" si="1">F3+5</f>
         <v>5</v>
       </c>
       <c r="G4">

</xml_diff>

<commit_message>
working combat through to death.
</commit_message>
<xml_diff>
--- a/Resources/Game_Data.xlsx
+++ b/Resources/Game_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="336" windowWidth="19920" windowHeight="8220" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="336" windowWidth="19920" windowHeight="8220" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Experience" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="164">
   <si>
     <t>Level</t>
   </si>
@@ -510,15 +510,17 @@
   <si>
     <t>longsword</t>
   </si>
+  <si>
+    <t>None</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;???_);_(@_)"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -1071,7 +1073,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1083,7 +1085,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2486,11 +2487,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="262278528"/>
-        <c:axId val="262296704"/>
+        <c:axId val="146738176"/>
+        <c:axId val="146756352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="262278528"/>
+        <c:axId val="146738176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2499,7 +2500,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="262296704"/>
+        <c:crossAx val="146756352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2507,7 +2508,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="262296704"/>
+        <c:axId val="146756352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2518,7 +2519,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="262278528"/>
+        <c:crossAx val="146738176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3855,11 +3856,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="262596480"/>
-        <c:axId val="262598016"/>
+        <c:axId val="199943680"/>
+        <c:axId val="199945216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="262596480"/>
+        <c:axId val="199943680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3869,7 +3870,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="262598016"/>
+        <c:crossAx val="199945216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3877,7 +3878,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="262598016"/>
+        <c:axId val="199945216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3888,7 +3889,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="262596480"/>
+        <c:crossAx val="199943680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6379,11 +6380,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="262635904"/>
-        <c:axId val="262637440"/>
+        <c:axId val="199983104"/>
+        <c:axId val="199984640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="262635904"/>
+        <c:axId val="199983104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6392,7 +6393,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="262637440"/>
+        <c:crossAx val="199984640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6400,7 +6401,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="262637440"/>
+        <c:axId val="199984640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6411,7 +6412,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="262635904"/>
+        <c:crossAx val="199983104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -26435,8 +26436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -47757,10 +47758,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L11:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -47769,210 +47770,263 @@
     <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" t="s">
         <v>147</v>
       </c>
-      <c r="B1" t="s">
-        <v>148</v>
-      </c>
       <c r="C1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" t="s">
         <v>149</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>150</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>151</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>152</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2">
+        <v>0.2</v>
+      </c>
+      <c r="D2">
+        <v>0.18</v>
+      </c>
+      <c r="E2">
+        <v>0.08</v>
+      </c>
+      <c r="F2">
+        <v>0.05</v>
+      </c>
+      <c r="G2">
+        <v>0.03</v>
+      </c>
+      <c r="H2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" t="s">
         <v>155</v>
       </c>
-      <c r="B2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C2" s="11">
+      <c r="C3">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="D3">
         <v>0.2</v>
       </c>
-      <c r="D2" s="11">
+      <c r="E3">
         <v>0.1</v>
       </c>
-      <c r="E2" s="11">
+      <c r="F3">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F2" s="11">
+      <c r="G3">
         <v>0.06</v>
       </c>
-      <c r="G2" s="11">
+      <c r="H3">
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" t="s">
         <v>155</v>
       </c>
-      <c r="B3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C3" s="11">
+      <c r="C4">
+        <v>0.35</v>
+      </c>
+      <c r="D4">
         <v>0.32500000000000001</v>
       </c>
-      <c r="D3" s="11">
+      <c r="E4">
         <v>0.22500000000000001</v>
       </c>
-      <c r="E3" s="11">
+      <c r="F4">
         <v>0.125</v>
       </c>
-      <c r="F3" s="11">
+      <c r="G4">
         <v>0.125</v>
       </c>
-      <c r="G3" s="11">
+      <c r="H4">
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" t="s">
         <v>155</v>
       </c>
-      <c r="B4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C4" s="11">
+      <c r="C5">
+        <v>0.4</v>
+      </c>
+      <c r="D5">
         <v>0.35</v>
       </c>
-      <c r="D4" s="11">
+      <c r="E5">
         <v>0.24</v>
       </c>
-      <c r="E4" s="11">
+      <c r="F5">
         <v>0.2</v>
       </c>
-      <c r="F4" s="11">
+      <c r="G5">
         <v>0.15</v>
       </c>
-      <c r="G4" s="11">
+      <c r="H5">
         <v>0.125</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" t="s">
         <v>155</v>
       </c>
-      <c r="B5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C5" s="11">
+      <c r="C6">
+        <v>0.4</v>
+      </c>
+      <c r="D6">
         <v>0.35</v>
       </c>
-      <c r="D5" s="11">
+      <c r="E6">
         <v>0.27500000000000002</v>
       </c>
-      <c r="E5" s="11">
+      <c r="F6">
         <v>0.22500000000000001</v>
       </c>
-      <c r="F5" s="11">
+      <c r="G6">
         <v>0.2</v>
       </c>
-      <c r="G5" s="11">
+      <c r="H6">
         <v>0.17499999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" t="s">
         <v>155</v>
       </c>
-      <c r="B6" t="s">
-        <v>161</v>
-      </c>
-      <c r="C6" s="11">
+      <c r="C7">
+        <v>0.45</v>
+      </c>
+      <c r="D7">
         <v>0.4</v>
       </c>
-      <c r="D6" s="11">
+      <c r="E7">
         <v>0.3</v>
       </c>
-      <c r="E6" s="11">
+      <c r="F7">
         <v>0.25</v>
       </c>
-      <c r="F6" s="11">
+      <c r="G7">
         <v>0.22500000000000001</v>
       </c>
-      <c r="G6" s="11">
+      <c r="H7">
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8" t="s">
         <v>155</v>
       </c>
-      <c r="B7" t="s">
-        <v>157</v>
-      </c>
-      <c r="C7" s="11">
+      <c r="C8">
+        <v>0.5</v>
+      </c>
+      <c r="D8">
         <v>0.45</v>
       </c>
-      <c r="D7" s="11">
+      <c r="E8">
         <v>0.32500000000000001</v>
       </c>
-      <c r="E7" s="11">
+      <c r="F8">
         <v>0.27500000000000002</v>
       </c>
-      <c r="F7" s="11">
+      <c r="G8">
         <v>0.25</v>
       </c>
-      <c r="G7" s="11">
+      <c r="H8">
         <v>0.18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9" t="s">
         <v>155</v>
       </c>
-      <c r="B8" t="s">
-        <v>159</v>
-      </c>
-      <c r="C8" s="11">
+      <c r="C9">
+        <v>0.5</v>
+      </c>
+      <c r="D9">
         <v>0.42</v>
       </c>
-      <c r="D8" s="11">
+      <c r="E9">
         <v>0.3</v>
       </c>
-      <c r="E8" s="11">
+      <c r="F9">
         <v>0.27</v>
       </c>
-      <c r="F8" s="11">
+      <c r="G9">
         <v>0.24</v>
       </c>
-      <c r="G8" s="11">
+      <c r="H9">
         <v>0.21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>160</v>
+      </c>
+      <c r="B10" t="s">
         <v>155</v>
       </c>
-      <c r="B9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C9" s="11">
+      <c r="C10">
+        <v>0.5</v>
+      </c>
+      <c r="D10">
         <v>0.45</v>
       </c>
-      <c r="D9" s="11">
+      <c r="E10">
         <v>0.32500000000000001</v>
       </c>
-      <c r="E9" s="11">
+      <c r="F10">
         <v>0.3</v>
       </c>
-      <c r="F9" s="11">
+      <c r="G10">
         <v>0.27500000000000002</v>
       </c>
-      <c r="G9" s="11">
+      <c r="H10">
         <v>0.25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
skills mental and physical points incorporated
</commit_message>
<xml_diff>
--- a/Resources/Game_Data.xlsx
+++ b/Resources/Game_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="336" windowWidth="19920" windowHeight="8220" firstSheet="4" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="336" windowWidth="19920" windowHeight="8220" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Experience" sheetId="1" r:id="rId1"/>
@@ -13,18 +13,19 @@
     <sheet name="Races" sheetId="3" r:id="rId4"/>
     <sheet name="Professions" sheetId="6" r:id="rId5"/>
     <sheet name="Attributes" sheetId="4" r:id="rId6"/>
-    <sheet name="Skills_Bonus" sheetId="5" r:id="rId7"/>
-    <sheet name="Weapon_Attack_Factors" sheetId="9" r:id="rId8"/>
-    <sheet name="Weapon_Damage_Factors" sheetId="7" r:id="rId9"/>
-    <sheet name="Position_Factors" sheetId="10" r:id="rId10"/>
-    <sheet name="Stance_Factors" sheetId="11" r:id="rId11"/>
+    <sheet name="Skills_Costs" sheetId="12" r:id="rId7"/>
+    <sheet name="Skills_Bonus" sheetId="5" r:id="rId8"/>
+    <sheet name="Weapon_Attack_Factors" sheetId="9" r:id="rId9"/>
+    <sheet name="Weapon_Damage_Factors" sheetId="7" r:id="rId10"/>
+    <sheet name="Position_Factors" sheetId="10" r:id="rId11"/>
+    <sheet name="Stance_Factors" sheetId="11" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="145621" calcMode="manual" iterate="1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="189">
   <si>
     <t>Level</t>
   </si>
@@ -561,6 +562,36 @@
   </si>
   <si>
     <t>guarded</t>
+  </si>
+  <si>
+    <t>physical_points</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>mental_points</t>
+  </si>
+  <si>
+    <t>blunt_weapons</t>
+  </si>
+  <si>
+    <t>polearm_weapons</t>
+  </si>
+  <si>
+    <t>armor</t>
+  </si>
+  <si>
+    <t>shield</t>
+  </si>
+  <si>
+    <t>dodging</t>
+  </si>
+  <si>
+    <t>physical_fitness</t>
+  </si>
+  <si>
+    <t>perception</t>
   </si>
 </sst>
 </file>
@@ -2536,11 +2567,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="259923328"/>
-        <c:axId val="259933312"/>
+        <c:axId val="171820928"/>
+        <c:axId val="171822464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="259923328"/>
+        <c:axId val="171820928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2549,7 +2580,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="259933312"/>
+        <c:crossAx val="171822464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2557,7 +2588,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="259933312"/>
+        <c:axId val="171822464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2568,7 +2599,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="259923328"/>
+        <c:crossAx val="171820928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3905,11 +3936,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="290273152"/>
-        <c:axId val="290274688"/>
+        <c:axId val="132964736"/>
+        <c:axId val="132966272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="290273152"/>
+        <c:axId val="132964736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3919,7 +3950,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="290274688"/>
+        <c:crossAx val="132966272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3927,7 +3958,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="290274688"/>
+        <c:axId val="132966272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3938,7 +3969,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="290273152"/>
+        <c:crossAx val="132964736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6429,11 +6460,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="313753984"/>
-        <c:axId val="313755520"/>
+        <c:axId val="133040768"/>
+        <c:axId val="133046656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="313753984"/>
+        <c:axId val="133040768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6442,7 +6473,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="313755520"/>
+        <c:crossAx val="133046656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6450,7 +6481,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="313755520"/>
+        <c:axId val="133046656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6461,7 +6492,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="313753984"/>
+        <c:crossAx val="133040768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7797,7 +7828,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="28" spans="3:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C28">
         <v>26</v>
       </c>
@@ -8259,7 +8290,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="42" spans="3:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C42">
         <v>40</v>
       </c>
@@ -8292,7 +8323,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="43" spans="3:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C43">
         <v>41</v>
       </c>
@@ -8325,7 +8356,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="44" spans="3:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C44">
         <v>42</v>
       </c>
@@ -10283,6 +10314,287 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2">
+        <v>0.2</v>
+      </c>
+      <c r="D2">
+        <v>0.18</v>
+      </c>
+      <c r="E2">
+        <v>0.08</v>
+      </c>
+      <c r="F2">
+        <v>0.05</v>
+      </c>
+      <c r="G2">
+        <v>0.03</v>
+      </c>
+      <c r="H2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="D3">
+        <v>0.2</v>
+      </c>
+      <c r="E3">
+        <v>0.1</v>
+      </c>
+      <c r="F3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G3">
+        <v>0.06</v>
+      </c>
+      <c r="H3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4">
+        <v>0.35</v>
+      </c>
+      <c r="D4">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="E4">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="F4">
+        <v>0.125</v>
+      </c>
+      <c r="G4">
+        <v>0.125</v>
+      </c>
+      <c r="H4">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5">
+        <v>0.4</v>
+      </c>
+      <c r="D5">
+        <v>0.35</v>
+      </c>
+      <c r="E5">
+        <v>0.24</v>
+      </c>
+      <c r="F5">
+        <v>0.2</v>
+      </c>
+      <c r="G5">
+        <v>0.15</v>
+      </c>
+      <c r="H5">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6">
+        <v>0.4</v>
+      </c>
+      <c r="D6">
+        <v>0.35</v>
+      </c>
+      <c r="E6">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="F6">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="G6">
+        <v>0.2</v>
+      </c>
+      <c r="H6">
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7">
+        <v>0.45</v>
+      </c>
+      <c r="D7">
+        <v>0.4</v>
+      </c>
+      <c r="E7">
+        <v>0.3</v>
+      </c>
+      <c r="F7">
+        <v>0.25</v>
+      </c>
+      <c r="G7">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="H7">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8">
+        <v>0.5</v>
+      </c>
+      <c r="D8">
+        <v>0.45</v>
+      </c>
+      <c r="E8">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="F8">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="G8">
+        <v>0.25</v>
+      </c>
+      <c r="H8">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C9">
+        <v>0.5</v>
+      </c>
+      <c r="D9">
+        <v>0.42</v>
+      </c>
+      <c r="E9">
+        <v>0.3</v>
+      </c>
+      <c r="F9">
+        <v>0.27</v>
+      </c>
+      <c r="G9">
+        <v>0.24</v>
+      </c>
+      <c r="H9">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>160</v>
+      </c>
+      <c r="B10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10">
+        <v>0.5</v>
+      </c>
+      <c r="D10">
+        <v>0.45</v>
+      </c>
+      <c r="E10">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="F10">
+        <v>0.3</v>
+      </c>
+      <c r="G10">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="H10">
+        <v>0.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -10355,12 +10667,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10559,7 +10871,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="AK3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AT4" sqref="AT4"/>
+      <selection pane="bottomRight" activeCell="AW3" sqref="AW3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14773,7 +15085,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="3:50" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:50" x14ac:dyDescent="0.3">
       <c r="C30">
         <f>Experience!C28</f>
         <v>26</v>
@@ -14923,7 +15235,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="3:50" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:50" x14ac:dyDescent="0.3">
       <c r="C31">
         <f>Experience!C29</f>
         <v>27</v>
@@ -16873,7 +17185,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="3:50" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:50" x14ac:dyDescent="0.3">
       <c r="C44">
         <f>Experience!C42</f>
         <v>40</v>
@@ -17023,7 +17335,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="3:50" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:50" x14ac:dyDescent="0.3">
       <c r="C45">
         <f>Experience!C43</f>
         <v>41</v>
@@ -17173,7 +17485,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="3:50" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:50" x14ac:dyDescent="0.3">
       <c r="C46">
         <f>Experience!C44</f>
         <v>42</v>
@@ -26755,7 +27067,7 @@
   <dimension ref="A1:Q127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27724,7 +28036,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C28">
         <f>Experience!C27</f>
         <v>25</v>
@@ -28212,7 +28524,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C42">
         <f>Experience!C41</f>
         <v>39</v>
@@ -28246,7 +28558,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C43">
         <f>Experience!C42</f>
         <v>40</v>
@@ -28280,7 +28592,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C44">
         <f>Experience!C43</f>
         <v>41</v>
@@ -30339,10 +30651,127 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O403"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31523,7 +31952,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>25</v>
       </c>
@@ -32139,7 +32568,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B42">
         <v>39</v>
       </c>
@@ -32183,7 +32612,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="43" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B43">
         <v>40</v>
       </c>
@@ -32227,7 +32656,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="44" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B44">
         <v>41</v>
       </c>
@@ -48074,7 +48503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -48347,285 +48776,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G1" t="s">
-        <v>152</v>
-      </c>
-      <c r="H1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C2">
-        <v>0.2</v>
-      </c>
-      <c r="D2">
-        <v>0.18</v>
-      </c>
-      <c r="E2">
-        <v>0.08</v>
-      </c>
-      <c r="F2">
-        <v>0.05</v>
-      </c>
-      <c r="G2">
-        <v>0.03</v>
-      </c>
-      <c r="H2">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C3">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="D3">
-        <v>0.2</v>
-      </c>
-      <c r="E3">
-        <v>0.1</v>
-      </c>
-      <c r="F3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G3">
-        <v>0.06</v>
-      </c>
-      <c r="H3">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B4" t="s">
-        <v>155</v>
-      </c>
-      <c r="C4">
-        <v>0.35</v>
-      </c>
-      <c r="D4">
-        <v>0.32500000000000001</v>
-      </c>
-      <c r="E4">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="F4">
-        <v>0.125</v>
-      </c>
-      <c r="G4">
-        <v>0.125</v>
-      </c>
-      <c r="H4">
-        <v>7.4999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C5">
-        <v>0.4</v>
-      </c>
-      <c r="D5">
-        <v>0.35</v>
-      </c>
-      <c r="E5">
-        <v>0.24</v>
-      </c>
-      <c r="F5">
-        <v>0.2</v>
-      </c>
-      <c r="G5">
-        <v>0.15</v>
-      </c>
-      <c r="H5">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>162</v>
-      </c>
-      <c r="B6" t="s">
-        <v>155</v>
-      </c>
-      <c r="C6">
-        <v>0.4</v>
-      </c>
-      <c r="D6">
-        <v>0.35</v>
-      </c>
-      <c r="E6">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="F6">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="G6">
-        <v>0.2</v>
-      </c>
-      <c r="H6">
-        <v>0.17499999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>161</v>
-      </c>
-      <c r="B7" t="s">
-        <v>155</v>
-      </c>
-      <c r="C7">
-        <v>0.45</v>
-      </c>
-      <c r="D7">
-        <v>0.4</v>
-      </c>
-      <c r="E7">
-        <v>0.3</v>
-      </c>
-      <c r="F7">
-        <v>0.25</v>
-      </c>
-      <c r="G7">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="H7">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>157</v>
-      </c>
-      <c r="B8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C8">
-        <v>0.5</v>
-      </c>
-      <c r="D8">
-        <v>0.45</v>
-      </c>
-      <c r="E8">
-        <v>0.32500000000000001</v>
-      </c>
-      <c r="F8">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="G8">
-        <v>0.25</v>
-      </c>
-      <c r="H8">
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>159</v>
-      </c>
-      <c r="B9" t="s">
-        <v>155</v>
-      </c>
-      <c r="C9">
-        <v>0.5</v>
-      </c>
-      <c r="D9">
-        <v>0.42</v>
-      </c>
-      <c r="E9">
-        <v>0.3</v>
-      </c>
-      <c r="F9">
-        <v>0.27</v>
-      </c>
-      <c r="G9">
-        <v>0.24</v>
-      </c>
-      <c r="H9">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>160</v>
-      </c>
-      <c r="B10" t="s">
-        <v>155</v>
-      </c>
-      <c r="C10">
-        <v>0.5</v>
-      </c>
-      <c r="D10">
-        <v>0.45</v>
-      </c>
-      <c r="E10">
-        <v>0.32500000000000001</v>
-      </c>
-      <c r="F10">
-        <v>0.3</v>
-      </c>
-      <c r="G10">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="H10">
-        <v>0.25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added mechanics for blunt and polearm weapons
</commit_message>
<xml_diff>
--- a/Resources/Game_Data.xlsx
+++ b/Resources/Game_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="336" windowWidth="19920" windowHeight="8220" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="336" windowWidth="19920" windowHeight="8220" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Experience" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="202">
   <si>
     <t>Level</t>
   </si>
@@ -592,6 +592,45 @@
   </si>
   <si>
     <t>perception</t>
+  </si>
+  <si>
+    <t>whip</t>
+  </si>
+  <si>
+    <t>mace</t>
+  </si>
+  <si>
+    <t>morning_star</t>
+  </si>
+  <si>
+    <t>flail</t>
+  </si>
+  <si>
+    <t>hammer</t>
+  </si>
+  <si>
+    <t>maul</t>
+  </si>
+  <si>
+    <t>cudgel</t>
+  </si>
+  <si>
+    <t>pilum</t>
+  </si>
+  <si>
+    <t>spear</t>
+  </si>
+  <si>
+    <t>halberd</t>
+  </si>
+  <si>
+    <t>trident</t>
+  </si>
+  <si>
+    <t>minimum_round_time</t>
+  </si>
+  <si>
+    <t>base_round_time</t>
   </si>
 </sst>
 </file>
@@ -2567,11 +2606,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="171820928"/>
-        <c:axId val="171822464"/>
+        <c:axId val="256787584"/>
+        <c:axId val="256789120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="171820928"/>
+        <c:axId val="256787584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2580,7 +2619,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171822464"/>
+        <c:crossAx val="256789120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2588,7 +2627,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="171822464"/>
+        <c:axId val="256789120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2599,7 +2638,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171820928"/>
+        <c:crossAx val="256787584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3936,11 +3975,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="132964736"/>
-        <c:axId val="132966272"/>
+        <c:axId val="288562560"/>
+        <c:axId val="288597120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="132964736"/>
+        <c:axId val="288562560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3950,7 +3989,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132966272"/>
+        <c:crossAx val="288597120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3958,7 +3997,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="132966272"/>
+        <c:axId val="288597120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3969,7 +4008,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132964736"/>
+        <c:crossAx val="288562560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6460,11 +6499,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="133040768"/>
-        <c:axId val="133046656"/>
+        <c:axId val="288675712"/>
+        <c:axId val="288677248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133040768"/>
+        <c:axId val="288675712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6473,7 +6512,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133046656"/>
+        <c:crossAx val="288677248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6481,7 +6520,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133046656"/>
+        <c:axId val="288677248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6492,7 +6531,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133040768"/>
+        <c:crossAx val="288675712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10318,7 +10357,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30653,8 +30692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30770,7 +30809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O403"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -48505,15 +48544,20 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>148</v>
       </c>
@@ -48538,8 +48582,14 @@
       <c r="H1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>201</v>
+      </c>
+      <c r="J1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>163</v>
       </c>
@@ -48564,8 +48614,14 @@
       <c r="H2">
         <v>-20</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>154</v>
       </c>
@@ -48590,8 +48646,14 @@
       <c r="H3">
         <v>-18</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>158</v>
       </c>
@@ -48616,8 +48678,14 @@
       <c r="H4">
         <v>-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>156</v>
       </c>
@@ -48642,8 +48710,14 @@
       <c r="H5">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>162</v>
       </c>
@@ -48668,8 +48742,14 @@
       <c r="H6">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>161</v>
       </c>
@@ -48694,8 +48774,14 @@
       <c r="H7">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>157</v>
       </c>
@@ -48720,8 +48806,14 @@
       <c r="H8">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>8</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>159</v>
       </c>
@@ -48746,8 +48838,14 @@
       <c r="H9">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>160</v>
       </c>
@@ -48771,6 +48869,364 @@
       </c>
       <c r="H10">
         <v>25</v>
+      </c>
+      <c r="I10">
+        <v>6</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>189</v>
+      </c>
+      <c r="B11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11">
+        <v>35</v>
+      </c>
+      <c r="D11">
+        <v>35</v>
+      </c>
+      <c r="E11">
+        <v>23</v>
+      </c>
+      <c r="F11">
+        <v>16</v>
+      </c>
+      <c r="G11">
+        <v>17</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>18</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
+      <c r="G12">
+        <v>24</v>
+      </c>
+      <c r="H12">
+        <v>17</v>
+      </c>
+      <c r="I12">
+        <v>4</v>
+      </c>
+      <c r="J12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>190</v>
+      </c>
+      <c r="B13" t="s">
+        <v>182</v>
+      </c>
+      <c r="C13">
+        <v>31</v>
+      </c>
+      <c r="D13">
+        <v>31</v>
+      </c>
+      <c r="E13">
+        <v>30</v>
+      </c>
+      <c r="F13">
+        <v>31</v>
+      </c>
+      <c r="G13">
+        <v>34</v>
+      </c>
+      <c r="H13">
+        <v>24</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="J13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>191</v>
+      </c>
+      <c r="B14" t="s">
+        <v>182</v>
+      </c>
+      <c r="C14">
+        <v>33</v>
+      </c>
+      <c r="D14">
+        <v>33</v>
+      </c>
+      <c r="E14">
+        <v>33</v>
+      </c>
+      <c r="F14">
+        <v>30</v>
+      </c>
+      <c r="G14">
+        <v>34</v>
+      </c>
+      <c r="H14">
+        <v>25</v>
+      </c>
+      <c r="I14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>18</v>
+      </c>
+      <c r="F15">
+        <v>23</v>
+      </c>
+      <c r="G15">
+        <v>27</v>
+      </c>
+      <c r="H15">
+        <v>18</v>
+      </c>
+      <c r="I15">
+        <v>6</v>
+      </c>
+      <c r="J15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>193</v>
+      </c>
+      <c r="B16" t="s">
+        <v>182</v>
+      </c>
+      <c r="C16">
+        <v>25</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+      <c r="E16">
+        <v>28</v>
+      </c>
+      <c r="F16">
+        <v>28</v>
+      </c>
+      <c r="G16">
+        <v>33</v>
+      </c>
+      <c r="H16">
+        <v>25</v>
+      </c>
+      <c r="I16">
+        <v>6</v>
+      </c>
+      <c r="J16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>194</v>
+      </c>
+      <c r="B17" t="s">
+        <v>182</v>
+      </c>
+      <c r="C17">
+        <v>25</v>
+      </c>
+      <c r="D17">
+        <v>25</v>
+      </c>
+      <c r="E17">
+        <v>30</v>
+      </c>
+      <c r="F17">
+        <v>34</v>
+      </c>
+      <c r="G17">
+        <v>38</v>
+      </c>
+      <c r="H17">
+        <v>27</v>
+      </c>
+      <c r="I17">
+        <v>7</v>
+      </c>
+      <c r="J17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>196</v>
+      </c>
+      <c r="B18" t="s">
+        <v>183</v>
+      </c>
+      <c r="C18">
+        <v>30</v>
+      </c>
+      <c r="D18">
+        <v>30</v>
+      </c>
+      <c r="E18">
+        <v>25</v>
+      </c>
+      <c r="F18">
+        <v>18</v>
+      </c>
+      <c r="G18">
+        <v>15</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>197</v>
+      </c>
+      <c r="B19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C19">
+        <v>33</v>
+      </c>
+      <c r="D19">
+        <v>33</v>
+      </c>
+      <c r="E19">
+        <v>30</v>
+      </c>
+      <c r="F19">
+        <v>30</v>
+      </c>
+      <c r="G19">
+        <v>28</v>
+      </c>
+      <c r="H19">
+        <v>21</v>
+      </c>
+      <c r="I19">
+        <v>6</v>
+      </c>
+      <c r="J19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B20" t="s">
+        <v>183</v>
+      </c>
+      <c r="C20">
+        <v>30</v>
+      </c>
+      <c r="D20">
+        <v>30</v>
+      </c>
+      <c r="E20">
+        <v>28</v>
+      </c>
+      <c r="F20">
+        <v>27</v>
+      </c>
+      <c r="G20">
+        <v>24</v>
+      </c>
+      <c r="H20">
+        <v>20</v>
+      </c>
+      <c r="I20">
+        <v>6</v>
+      </c>
+      <c r="J20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>199</v>
+      </c>
+      <c r="B21" t="s">
+        <v>183</v>
+      </c>
+      <c r="C21">
+        <v>29</v>
+      </c>
+      <c r="D21">
+        <v>29</v>
+      </c>
+      <c r="E21">
+        <v>28</v>
+      </c>
+      <c r="F21">
+        <v>26</v>
+      </c>
+      <c r="G21">
+        <v>29</v>
+      </c>
+      <c r="H21">
+        <v>13</v>
+      </c>
+      <c r="I21">
+        <v>6</v>
+      </c>
+      <c r="J21">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added weapons to the weaponsmith
</commit_message>
<xml_diff>
--- a/Resources/Game_Data.xlsx
+++ b/Resources/Game_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="336" windowWidth="19920" windowHeight="8220" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="336" windowWidth="19920" windowHeight="8220" firstSheet="7" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Experience" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,14 @@
     <sheet name="Weapon_Damage_Factors" sheetId="7" r:id="rId10"/>
     <sheet name="Position_Factors" sheetId="10" r:id="rId11"/>
     <sheet name="Stance_Factors" sheetId="11" r:id="rId12"/>
+    <sheet name="Material_Factors" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="206">
   <si>
     <t>Level</t>
   </si>
@@ -631,6 +632,18 @@
   </si>
   <si>
     <t>base_round_time</t>
+  </si>
+  <si>
+    <t>handaxe</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>Iron</t>
+  </si>
+  <si>
+    <t>Steel</t>
   </si>
 </sst>
 </file>
@@ -2606,11 +2619,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="256787584"/>
-        <c:axId val="256789120"/>
+        <c:axId val="247551104"/>
+        <c:axId val="247552640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="256787584"/>
+        <c:axId val="247551104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2619,7 +2632,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="256789120"/>
+        <c:crossAx val="247552640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2627,7 +2640,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="256789120"/>
+        <c:axId val="247552640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2638,7 +2651,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="256787584"/>
+        <c:crossAx val="247551104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3975,11 +3988,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="288562560"/>
-        <c:axId val="288597120"/>
+        <c:axId val="126360960"/>
+        <c:axId val="247166080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="288562560"/>
+        <c:axId val="126360960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3989,7 +4002,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="288597120"/>
+        <c:crossAx val="247166080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3997,7 +4010,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288597120"/>
+        <c:axId val="247166080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4008,7 +4021,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="288562560"/>
+        <c:crossAx val="126360960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6499,11 +6512,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="288675712"/>
-        <c:axId val="288677248"/>
+        <c:axId val="246265728"/>
+        <c:axId val="246267264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="288675712"/>
+        <c:axId val="246265728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6512,7 +6525,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="288677248"/>
+        <c:crossAx val="246267264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6520,7 +6533,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288677248"/>
+        <c:axId val="246267264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6531,7 +6544,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="288675712"/>
+        <c:crossAx val="246265728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10787,6 +10800,36 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
@@ -48547,7 +48590,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -48815,7 +48858,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>202</v>
       </c>
       <c r="B9" t="s">
         <v>155</v>

</xml_diff>

<commit_message>
the program is messed right now. in the middle of implementing socketio.
</commit_message>
<xml_diff>
--- a/Resources/Game_Data.xlsx
+++ b/Resources/Game_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="336" windowWidth="19920" windowHeight="8220" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="336" windowWidth="19920" windowHeight="8220" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Experience" sheetId="1" r:id="rId1"/>
@@ -2619,11 +2619,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="247551104"/>
-        <c:axId val="247552640"/>
+        <c:axId val="434576384"/>
+        <c:axId val="434590464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="247551104"/>
+        <c:axId val="434576384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2632,7 +2632,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="247552640"/>
+        <c:crossAx val="434590464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2640,7 +2640,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="247552640"/>
+        <c:axId val="434590464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2651,7 +2651,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="247551104"/>
+        <c:crossAx val="434576384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3028,7 +3028,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>32.5</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>38.5</c:v>
@@ -3671,7 +3671,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>32</c:v>
@@ -3988,11 +3988,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="126360960"/>
-        <c:axId val="247166080"/>
+        <c:axId val="380708352"/>
+        <c:axId val="380709888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="126360960"/>
+        <c:axId val="380708352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4002,7 +4002,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="247166080"/>
+        <c:crossAx val="380709888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4010,7 +4010,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="247166080"/>
+        <c:axId val="380709888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4021,7 +4021,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126360960"/>
+        <c:crossAx val="380708352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6512,11 +6512,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="246265728"/>
-        <c:axId val="246267264"/>
+        <c:axId val="381251584"/>
+        <c:axId val="381253120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="246265728"/>
+        <c:axId val="381251584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6525,7 +6525,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="246267264"/>
+        <c:crossAx val="381253120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6533,7 +6533,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246267264"/>
+        <c:axId val="381253120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6544,7 +6544,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="246265728"/>
+        <c:crossAx val="381251584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10949,11 +10949,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX104"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="AK3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AW3" sqref="AW3"/>
+      <selection pane="bottomRight" activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11212,11 +11212,11 @@
         <v>35</v>
       </c>
       <c r="E3">
+        <f>$N$4/8</f>
+        <v>66</v>
+      </c>
+      <c r="F3">
         <f t="shared" ref="E3:L3" si="0">$N$4/8</f>
-        <v>66</v>
-      </c>
-      <c r="F3">
-        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="G3">
@@ -11302,8 +11302,8 @@
         <v>0</v>
       </c>
       <c r="R4">
-        <f>ROUND((E4-$E$3)/2+INDEX(Races!$C$3:$J$14,MATCH('Stat Growth'!$A$2,Races!$A$3:$A$14,0),MATCH('Stat Growth'!R$2,Races!$C$2:$J$2,0)),0)</f>
-        <v>5</v>
+        <f>ROUND((E4-$E$3)/2+INDEX(Races!$C$3:$J$14,MATCH('Stat Growth'!$A$2,Races!$A$3:$A$14,0),MATCH('Stat Growth'!R$2,Races!$C$2:$J$2,0)),0)*0</f>
+        <v>0</v>
       </c>
       <c r="S4">
         <f>ROUND((F4-$E$3)/2+INDEX(Races!$C$3:$J$14,MATCH('Stat Growth'!$A$2,Races!$A$3:$A$14,0),MATCH('Stat Growth'!S$2,Races!$C$2:$J$2,0)),0)</f>
@@ -27224,11 +27224,11 @@
       </c>
       <c r="E3">
         <f>'Stat Growth'!R4</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <f>E3+Skills_Bonus!$D$4*Attributes!$A$3+INDEX(Skills_Bonus!D3:D403,MATCH(C3*$A$3,Skills_Bonus!$B$3:$B$403))</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H3">
         <f>'Stat Growth'!U4+'Stat Growth'!V4/4+$A$24*Skills_Bonus!$L$4+Attributes!C3*Attributes!$A$24</f>
@@ -27236,15 +27236,15 @@
       </c>
       <c r="J3">
         <f>'Stat Growth'!R4/4+'Stat Growth'!T4/4+Skills_Bonus!$K$4*Attributes!$A$21+Attributes!$A$21*Attributes!C3</f>
-        <v>11.25</v>
+        <v>10</v>
       </c>
       <c r="L3">
         <f>'Stat Growth'!R4/4+'Stat Growth'!T4/4+Skills_Bonus!$D$4*Attributes!$A$3+Attributes!C3*Attributes!$A$3</f>
-        <v>11.25</v>
+        <v>10</v>
       </c>
       <c r="N3">
         <f>H3+J3+L3</f>
-        <v>32.5</v>
+        <v>30</v>
       </c>
       <c r="P3">
         <f>TRUNC(('Stat Growth'!E4+'Stat Growth'!F4)/10)</f>
@@ -30853,7 +30853,7 @@
   <dimension ref="A1:O403"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -48589,7 +48589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>

</xml_diff>